<commit_message>
Saving the corresponding LibreOffice file as an Excel file in 3-ipip-300_item-NEO/ipip-300_items-NEO.xlsx .
</commit_message>
<xml_diff>
--- a/questionnaires/3-ipip-300_item-NEO/ipip-300_items-NEO.xlsx
+++ b/questionnaires/3-ipip-300_item-NEO/ipip-300_items-NEO.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="ipip-300_items-NEO" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Score Values for .csv" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="362">
   <si>
     <t xml:space="preserve">IPIP 300 Item NEO-PI-R Open Source Questionnaire</t>
   </si>
@@ -1127,6 +1128,9 @@
   </si>
   <si>
     <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use right-click → Paste Special → Paste Special… to paste just the score here, then use File → Save As… to save that as a .csv file</t>
   </si>
 </sst>
 </file>
@@ -1283,7 +1287,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1356,7 +1360,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1368,7 +1372,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1376,8 +1380,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1480,9 +1492,9 @@
   <dimension ref="A1:P700"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A311" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="F345" activeCellId="0" sqref="F345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14010,11 +14022,11 @@
         <v>0</v>
       </c>
       <c r="E313" s="17" t="n">
-        <f aca="false">QUOTIENT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D313,30),3)</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT(D313,60),5),12)</f>
+        <v>-25</v>
       </c>
       <c r="F313" s="18" t="str">
-        <f aca="false">IF(E313&lt;=20,"Very Low",IF(E313&lt;=40,"Low",IF(E313&lt;60,"Average",IF(E313&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E313&lt;=20,"Very Low",IF(E313&lt;=36,"Low",IF(E313&lt;=46,"A Little Low",IF(E313&lt;=53,"Average",IF(E313&lt;=63,"A Little High",IF(E313&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
       <c r="O313" s="4"/>
@@ -14030,11 +14042,11 @@
         <v>0</v>
       </c>
       <c r="E314" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D314,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D314,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F314" s="21" t="str">
-        <f aca="false">IF(E314&lt;=20,"Very Low",IF(E314&lt;=40,"Low",IF(E314&lt;60,"Average",IF(E314&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E314&lt;=20,"Very Low",IF(E314&lt;=36,"Low",IF(E314&lt;=46,"A Little Low",IF(E314&lt;=53,"Average",IF(E314&lt;=63,"A Little High",IF(E314&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
       <c r="O314" s="4"/>
@@ -14050,11 +14062,11 @@
         <v>0</v>
       </c>
       <c r="E315" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D315,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D315,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F315" s="21" t="str">
-        <f aca="false">IF(E315&lt;=20,"Very Low",IF(E315&lt;=40,"Low",IF(E315&lt;60,"Average",IF(E315&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E315&lt;=20,"Very Low",IF(E315&lt;=36,"Low",IF(E315&lt;=46,"A Little Low",IF(E315&lt;=53,"Average",IF(E315&lt;=63,"A Little High",IF(E315&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
       <c r="O315" s="4"/>
@@ -14070,11 +14082,11 @@
         <v>0</v>
       </c>
       <c r="E316" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D316,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D316,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F316" s="21" t="str">
-        <f aca="false">IF(E316&lt;=20,"Very Low",IF(E316&lt;=40,"Low",IF(E316&lt;60,"Average",IF(E316&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E316&lt;=20,"Very Low",IF(E316&lt;=36,"Low",IF(E316&lt;=46,"A Little Low",IF(E316&lt;=53,"Average",IF(E316&lt;=63,"A Little High",IF(E316&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
       <c r="O316" s="4"/>
@@ -14090,11 +14102,11 @@
         <v>0</v>
       </c>
       <c r="E317" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D317,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D317,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F317" s="21" t="str">
-        <f aca="false">IF(E317&lt;=20,"Very Low",IF(E317&lt;=40,"Low",IF(E317&lt;60,"Average",IF(E317&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E317&lt;=20,"Very Low",IF(E317&lt;=36,"Low",IF(E317&lt;=46,"A Little Low",IF(E317&lt;=53,"Average",IF(E317&lt;=63,"A Little High",IF(E317&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
       <c r="O317" s="4"/>
@@ -14110,11 +14122,11 @@
         <v>0</v>
       </c>
       <c r="E318" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D318,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D318,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F318" s="21" t="str">
-        <f aca="false">IF(E318&lt;=20,"Very Low",IF(E318&lt;=40,"Low",IF(E318&lt;60,"Average",IF(E318&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E318&lt;=20,"Very Low",IF(E318&lt;=36,"Low",IF(E318&lt;=46,"A Little Low",IF(E318&lt;=53,"Average",IF(E318&lt;=63,"A Little High",IF(E318&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
       <c r="O318" s="4"/>
@@ -14130,11 +14142,11 @@
         <v>0</v>
       </c>
       <c r="E319" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D319,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D319,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F319" s="21" t="str">
-        <f aca="false">IF(E319&lt;=20,"Very Low",IF(E319&lt;=40,"Low",IF(E319&lt;60,"Average",IF(E319&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E319&lt;=20,"Very Low",IF(E319&lt;=36,"Low",IF(E319&lt;=46,"A Little Low",IF(E319&lt;=53,"Average",IF(E319&lt;=63,"A Little High",IF(E319&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14144,7 +14156,7 @@
       <c r="C320" s="10"/>
       <c r="D320" s="2"/>
       <c r="E320" s="2"/>
-      <c r="F320" s="21"/>
+      <c r="F320" s="23"/>
     </row>
     <row r="321" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="15" t="s">
@@ -14157,11 +14169,11 @@
         <v>0</v>
       </c>
       <c r="E321" s="17" t="n">
-        <f aca="false">QUOTIENT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D321,30),3)</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT(D321,60),5),12)</f>
+        <v>-25</v>
       </c>
       <c r="F321" s="18" t="str">
-        <f aca="false">IF(E321&lt;=20,"Very Low",IF(E321&lt;=40,"Low",IF(E321&lt;60,"Average",IF(E321&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E321&lt;=20,"Very Low",IF(E321&lt;=36,"Low",IF(E321&lt;=46,"A Little Low",IF(E321&lt;=53,"Average",IF(E321&lt;=63,"A Little High",IF(E321&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14176,11 +14188,11 @@
         <v>0</v>
       </c>
       <c r="E322" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D322,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D322,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F322" s="21" t="str">
-        <f aca="false">IF(E322&lt;=20,"Very Low",IF(E322&lt;=40,"Low",IF(E322&lt;60,"Average",IF(E322&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E322&lt;=20,"Very Low",IF(E322&lt;=36,"Low",IF(E322&lt;=46,"A Little Low",IF(E322&lt;=53,"Average",IF(E322&lt;=63,"A Little High",IF(E322&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14195,11 +14207,11 @@
         <v>0</v>
       </c>
       <c r="E323" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D323,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D323,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F323" s="21" t="str">
-        <f aca="false">IF(E323&lt;=20,"Very Low",IF(E323&lt;=40,"Low",IF(E323&lt;60,"Average",IF(E323&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E323&lt;=20,"Very Low",IF(E323&lt;=36,"Low",IF(E323&lt;=46,"A Little Low",IF(E323&lt;=53,"Average",IF(E323&lt;=63,"A Little High",IF(E323&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14214,11 +14226,11 @@
         <v>0</v>
       </c>
       <c r="E324" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D324,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D324,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F324" s="21" t="str">
-        <f aca="false">IF(E324&lt;=20,"Very Low",IF(E324&lt;=40,"Low",IF(E324&lt;60,"Average",IF(E324&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E324&lt;=20,"Very Low",IF(E324&lt;=36,"Low",IF(E324&lt;=46,"A Little Low",IF(E324&lt;=53,"Average",IF(E324&lt;=63,"A Little High",IF(E324&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14233,11 +14245,11 @@
         <v>0</v>
       </c>
       <c r="E325" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D325,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D325,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F325" s="21" t="str">
-        <f aca="false">IF(E325&lt;=20,"Very Low",IF(E325&lt;=40,"Low",IF(E325&lt;60,"Average",IF(E325&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E325&lt;=20,"Very Low",IF(E325&lt;=36,"Low",IF(E325&lt;=46,"A Little Low",IF(E325&lt;=53,"Average",IF(E325&lt;=63,"A Little High",IF(E325&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14252,11 +14264,11 @@
         <v>0</v>
       </c>
       <c r="E326" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D326,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D326,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F326" s="21" t="str">
-        <f aca="false">IF(E326&lt;=20,"Very Low",IF(E326&lt;=40,"Low",IF(E326&lt;60,"Average",IF(E326&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E326&lt;=20,"Very Low",IF(E326&lt;=36,"Low",IF(E326&lt;=46,"A Little Low",IF(E326&lt;=53,"Average",IF(E326&lt;=63,"A Little High",IF(E326&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14271,11 +14283,11 @@
         <v>0</v>
       </c>
       <c r="E327" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D327,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D327,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F327" s="21" t="str">
-        <f aca="false">IF(E327&lt;=20,"Very Low",IF(E327&lt;=40,"Low",IF(E327&lt;60,"Average",IF(E327&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E327&lt;=20,"Very Low",IF(E327&lt;=36,"Low",IF(E327&lt;=46,"A Little Low",IF(E327&lt;=53,"Average",IF(E327&lt;=63,"A Little High",IF(E327&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14285,24 +14297,24 @@
       <c r="C328" s="10"/>
       <c r="D328" s="2"/>
       <c r="E328" s="2"/>
-      <c r="F328" s="21"/>
+      <c r="F328" s="23"/>
     </row>
     <row r="329" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="B329" s="23"/>
-      <c r="C329" s="23"/>
+      <c r="B329" s="24"/>
+      <c r="C329" s="24"/>
       <c r="D329" s="17" t="n">
         <f aca="false">SUM(D330:D335)</f>
         <v>0</v>
       </c>
       <c r="E329" s="17" t="n">
-        <f aca="false">QUOTIENT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D329,30),3)</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT(D329,60),5),12)</f>
+        <v>-25</v>
       </c>
       <c r="F329" s="18" t="str">
-        <f aca="false">IF(E329&lt;=20,"Very Low",IF(E329&lt;=40,"Low",IF(E329&lt;60,"Average",IF(E329&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E329&lt;=20,"Very Low",IF(E329&lt;=36,"Low",IF(E329&lt;=46,"A Little Low",IF(E329&lt;=53,"Average",IF(E329&lt;=63,"A Little High",IF(E329&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14317,11 +14329,11 @@
         <v>0</v>
       </c>
       <c r="E330" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D330,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D330,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F330" s="21" t="str">
-        <f aca="false">IF(E330&lt;=20,"Very Low",IF(E330&lt;=40,"Low",IF(E330&lt;60,"Average",IF(E330&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E330&lt;=20,"Very Low",IF(E330&lt;=36,"Low",IF(E330&lt;=46,"A Little Low",IF(E330&lt;=53,"Average",IF(E330&lt;=63,"A Little High",IF(E330&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14336,11 +14348,11 @@
         <v>0</v>
       </c>
       <c r="E331" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D331,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D331,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F331" s="21" t="str">
-        <f aca="false">IF(E331&lt;=20,"Very Low",IF(E331&lt;=40,"Low",IF(E331&lt;60,"Average",IF(E331&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E331&lt;=20,"Very Low",IF(E331&lt;=36,"Low",IF(E331&lt;=46,"A Little Low",IF(E331&lt;=53,"Average",IF(E331&lt;=63,"A Little High",IF(E331&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14355,11 +14367,11 @@
         <v>0</v>
       </c>
       <c r="E332" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D332,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D332,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F332" s="21" t="str">
-        <f aca="false">IF(E332&lt;=20,"Very Low",IF(E332&lt;=40,"Low",IF(E332&lt;60,"Average",IF(E332&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E332&lt;=20,"Very Low",IF(E332&lt;=36,"Low",IF(E332&lt;=46,"A Little Low",IF(E332&lt;=53,"Average",IF(E332&lt;=63,"A Little High",IF(E332&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14374,11 +14386,11 @@
         <v>0</v>
       </c>
       <c r="E333" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D333,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D333,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F333" s="21" t="str">
-        <f aca="false">IF(E333&lt;=20,"Very Low",IF(E333&lt;=40,"Low",IF(E333&lt;60,"Average",IF(E333&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E333&lt;=20,"Very Low",IF(E333&lt;=36,"Low",IF(E333&lt;=46,"A Little Low",IF(E333&lt;=53,"Average",IF(E333&lt;=63,"A Little High",IF(E333&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14393,11 +14405,11 @@
         <v>0</v>
       </c>
       <c r="E334" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D334,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D334,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F334" s="21" t="str">
-        <f aca="false">IF(E334&lt;=20,"Very Low",IF(E334&lt;=40,"Low",IF(E334&lt;60,"Average",IF(E334&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E334&lt;=20,"Very Low",IF(E334&lt;=36,"Low",IF(E334&lt;=46,"A Little Low",IF(E334&lt;=53,"Average",IF(E334&lt;=63,"A Little High",IF(E334&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14412,11 +14424,11 @@
         <v>0</v>
       </c>
       <c r="E335" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D335,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D335,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F335" s="21" t="str">
-        <f aca="false">IF(E335&lt;=20,"Very Low",IF(E335&lt;=40,"Low",IF(E335&lt;60,"Average",IF(E335&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E335&lt;=20,"Very Low",IF(E335&lt;=36,"Low",IF(E335&lt;=46,"A Little Low",IF(E335&lt;=53,"Average",IF(E335&lt;=63,"A Little High",IF(E335&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14426,24 +14438,24 @@
       <c r="C336" s="10"/>
       <c r="D336" s="17"/>
       <c r="E336" s="17"/>
-      <c r="F336" s="18"/>
+      <c r="F336" s="25"/>
     </row>
     <row r="337" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="24" t="s">
+      <c r="A337" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="B337" s="25"/>
-      <c r="C337" s="25"/>
+      <c r="B337" s="27"/>
+      <c r="C337" s="27"/>
       <c r="D337" s="17" t="n">
         <f aca="false">SUM(D338:D343)</f>
         <v>0</v>
       </c>
       <c r="E337" s="17" t="n">
-        <f aca="false">QUOTIENT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D337,30),3)</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT(D337,60),5),12)</f>
+        <v>-25</v>
       </c>
       <c r="F337" s="18" t="str">
-        <f aca="false">IF(E337&lt;=20,"Very Low",IF(E337&lt;=40,"Low",IF(E337&lt;60,"Average",IF(E337&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E337&lt;=20,"Very Low",IF(E337&lt;=36,"Low",IF(E337&lt;=46,"A Little Low",IF(E337&lt;=53,"Average",IF(E337&lt;=63,"A Little High",IF(E337&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14458,11 +14470,11 @@
         <v>0</v>
       </c>
       <c r="E338" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D338,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D338,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F338" s="21" t="str">
-        <f aca="false">IF(E338&lt;=20,"Very Low",IF(E338&lt;=40,"Low",IF(E338&lt;60,"Average",IF(E338&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E338&lt;=20,"Very Low",IF(E338&lt;=36,"Low",IF(E338&lt;=46,"A Little Low",IF(E338&lt;=53,"Average",IF(E338&lt;=63,"A Little High",IF(E338&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14477,11 +14489,11 @@
         <v>0</v>
       </c>
       <c r="E339" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D339,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D339,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F339" s="21" t="str">
-        <f aca="false">IF(E339&lt;=20,"Very Low",IF(E339&lt;=40,"Low",IF(E339&lt;60,"Average",IF(E339&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E339&lt;=20,"Very Low",IF(E339&lt;=36,"Low",IF(E339&lt;=46,"A Little Low",IF(E339&lt;=53,"Average",IF(E339&lt;=63,"A Little High",IF(E339&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14496,11 +14508,11 @@
         <v>0</v>
       </c>
       <c r="E340" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D340,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D340,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F340" s="21" t="str">
-        <f aca="false">IF(E340&lt;=20,"Very Low",IF(E340&lt;=40,"Low",IF(E340&lt;60,"Average",IF(E340&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E340&lt;=20,"Very Low",IF(E340&lt;=36,"Low",IF(E340&lt;=46,"A Little Low",IF(E340&lt;=53,"Average",IF(E340&lt;=63,"A Little High",IF(E340&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14515,11 +14527,11 @@
         <v>0</v>
       </c>
       <c r="E341" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D341,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D341,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F341" s="21" t="str">
-        <f aca="false">IF(E341&lt;=20,"Very Low",IF(E341&lt;=40,"Low",IF(E341&lt;60,"Average",IF(E341&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E341&lt;=20,"Very Low",IF(E341&lt;=36,"Low",IF(E341&lt;=46,"A Little Low",IF(E341&lt;=53,"Average",IF(E341&lt;=63,"A Little High",IF(E341&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14534,11 +14546,11 @@
         <v>0</v>
       </c>
       <c r="E342" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D342,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D342,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F342" s="21" t="str">
-        <f aca="false">IF(E342&lt;=20,"Very Low",IF(E342&lt;=40,"Low",IF(E342&lt;60,"Average",IF(E342&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E342&lt;=20,"Very Low",IF(E342&lt;=36,"Low",IF(E342&lt;=46,"A Little Low",IF(E342&lt;=53,"Average",IF(E342&lt;=63,"A Little High",IF(E342&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14553,11 +14565,11 @@
         <v>0</v>
       </c>
       <c r="E343" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D343,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D343,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F343" s="21" t="str">
-        <f aca="false">IF(E343&lt;=20,"Very Low",IF(E343&lt;=40,"Low",IF(E343&lt;60,"Average",IF(E343&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E343&lt;=20,"Very Low",IF(E343&lt;=36,"Low",IF(E343&lt;=46,"A Little Low",IF(E343&lt;=53,"Average",IF(E343&lt;=63,"A Little High",IF(E343&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14570,18 +14582,18 @@
       <c r="A345" s="15" t="s">
         <v>355</v>
       </c>
-      <c r="B345" s="23"/>
-      <c r="C345" s="23"/>
+      <c r="B345" s="24"/>
+      <c r="C345" s="24"/>
       <c r="D345" s="17" t="n">
         <f aca="false">SUM(D346:D351)</f>
         <v>0</v>
       </c>
       <c r="E345" s="17" t="n">
-        <f aca="false">QUOTIENT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D345,30),3)</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT(D345,60),5),12)</f>
+        <v>-25</v>
       </c>
       <c r="F345" s="18" t="str">
-        <f aca="false">IF(E345&lt;=20,"Very Low",IF(E345&lt;=40,"Low",IF(E345&lt;60,"Average",IF(E345&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E345&lt;=20,"Very Low",IF(E345&lt;=36,"Low",IF(E345&lt;=46,"A Little Low",IF(E345&lt;=53,"Average",IF(E345&lt;=63,"A Little High",IF(E345&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14596,11 +14608,11 @@
         <v>0</v>
       </c>
       <c r="E346" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D346,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D346,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F346" s="21" t="str">
-        <f aca="false">IF(E346&lt;=20,"Very Low",IF(E346&lt;=40,"Low",IF(E346&lt;60,"Average",IF(E346&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E346&lt;=20,"Very Low",IF(E346&lt;=36,"Low",IF(E346&lt;=46,"A Little Low",IF(E346&lt;=53,"Average",IF(E346&lt;=63,"A Little High",IF(E346&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14615,11 +14627,11 @@
         <v>0</v>
       </c>
       <c r="E347" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D347,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D347,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F347" s="21" t="str">
-        <f aca="false">IF(E347&lt;=20,"Very Low",IF(E347&lt;=40,"Low",IF(E347&lt;60,"Average",IF(E347&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E347&lt;=20,"Very Low",IF(E347&lt;=36,"Low",IF(E347&lt;=46,"A Little Low",IF(E347&lt;=53,"Average",IF(E347&lt;=63,"A Little High",IF(E347&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14634,11 +14646,11 @@
         <v>0</v>
       </c>
       <c r="E348" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D348,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D348,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F348" s="21" t="str">
-        <f aca="false">IF(E348&lt;=20,"Very Low",IF(E348&lt;=40,"Low",IF(E348&lt;60,"Average",IF(E348&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E348&lt;=20,"Very Low",IF(E348&lt;=36,"Low",IF(E348&lt;=46,"A Little Low",IF(E348&lt;=53,"Average",IF(E348&lt;=63,"A Little High",IF(E348&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14653,11 +14665,11 @@
         <v>0</v>
       </c>
       <c r="E349" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D349,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D349,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F349" s="21" t="str">
-        <f aca="false">IF(E349&lt;=20,"Very Low",IF(E349&lt;=40,"Low",IF(E349&lt;60,"Average",IF(E349&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E349&lt;=20,"Very Low",IF(E349&lt;=36,"Low",IF(E349&lt;=46,"A Little Low",IF(E349&lt;=53,"Average",IF(E349&lt;=63,"A Little High",IF(E349&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14672,11 +14684,11 @@
         <v>0</v>
       </c>
       <c r="E350" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D350,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D350,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F350" s="21" t="str">
-        <f aca="false">IF(E350&lt;=20,"Very Low",IF(E350&lt;=40,"Low",IF(E350&lt;60,"Average",IF(E350&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E350&lt;=20,"Very Low",IF(E350&lt;=36,"Low",IF(E350&lt;=46,"A Little Low",IF(E350&lt;=53,"Average",IF(E350&lt;=63,"A Little High",IF(E350&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -14691,19 +14703,19 @@
         <v>0</v>
       </c>
       <c r="E351" s="2" t="n">
-        <f aca="false">PRODUCT(2,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D351,5))</f>
-        <v>-10</v>
+        <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D351,10)),2)</f>
+        <v>-25</v>
       </c>
       <c r="F351" s="21" t="str">
-        <f aca="false">IF(E351&lt;=20,"Very Low",IF(E351&lt;=40,"Low",IF(E351&lt;60,"Average",IF(E351&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(E351&lt;=20,"Very Low",IF(E351&lt;=36,"Low",IF(E351&lt;=46,"A Little Low",IF(E351&lt;=53,"Average",IF(E351&lt;=63,"A Little High",IF(E351&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B352" s="26"/>
+      <c r="B352" s="28"/>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A360" s="27" t="s">
+      <c r="A360" s="29" t="s">
         <v>356</v>
       </c>
       <c r="B360" s="2" t="s">
@@ -14720,11 +14732,11 @@
       </c>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A400" s="28"/>
-      <c r="B400" s="28"/>
-      <c r="C400" s="28"/>
-      <c r="D400" s="28"/>
-      <c r="E400" s="28"/>
+      <c r="A400" s="30"/>
+      <c r="B400" s="30"/>
+      <c r="C400" s="30"/>
+      <c r="D400" s="30"/>
+      <c r="E400" s="30"/>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B402" s="2"/>
@@ -16579,4 +16591,33 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>361</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the Excel version in ipip-300_items-NEO.xlsx to contain the corresponding NEO-PI-R Facets.
</commit_message>
<xml_diff>
--- a/questionnaires/3-ipip-300_item-NEO/ipip-300_items-NEO.xlsx
+++ b/questionnaires/3-ipip-300_item-NEO/ipip-300_items-NEO.xlsx
@@ -21,9 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="360">
-  <si>
-    <t xml:space="preserve">IPIP 300 Item NEO-PI-R Open Source Questionnaire</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="394">
+  <si>
+    <t xml:space="preserve">IPIP 300 Item “NEO” Open Source Questionnaire</t>
   </si>
   <si>
     <t xml:space="preserve">Enter an “x” in Precisely One Column for Each Item</t>
@@ -1091,6 +1091,29 @@
     <t xml:space="preserve">Score:</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <u val="single"/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Factor/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">NEO-PI-R Facet¹</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">IPIP Facet²</t>
+  </si>
+  <si>
     <t xml:space="preserve">Raw</t>
   </si>
   <si>
@@ -1103,16 +1126,162 @@
     <t xml:space="preserve">Neuroticism </t>
   </si>
   <si>
+    <t xml:space="preserve">N2: Angry Hostility </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N1: Anxiety </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N3: Depression </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N5: Impulsiveness </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N4: Self-Consciousness </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N6: Vulnerability </t>
+  </si>
+  <si>
     <t xml:space="preserve">Extraversion </t>
   </si>
   <si>
+    <t xml:space="preserve">E4: Activity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E3: Assertiveness </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E6: Positive Emotions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E5: Excitement-Seeking </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1: Warmth </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E2: Gregariousness </t>
+  </si>
+  <si>
     <t xml:space="preserve">Openness </t>
   </si>
   <si>
+    <t xml:space="preserve">O4: Actions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O2: Aesthetics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O3: Feelings </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O1: Fantasy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O5: Ideas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O6: Values </t>
+  </si>
+  <si>
     <t xml:space="preserve">Agreeableness</t>
   </si>
   <si>
+    <t xml:space="preserve">A3: Altruism </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4: Compliance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5: Modesty </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2: Straightforwardness </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A6: Tender- Mindedness </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1: Trust </t>
+  </si>
+  <si>
     <t xml:space="preserve">Conscientiousness </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4: Achievement-Striving </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6: Deliberation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3: Dutifulness </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2: Order </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C5: Self-Discipline </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1: Competence</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">¹ NEO-PI-R Facets come from </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Personality and Adulthood</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> by Costa and McRae, 2003.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">² IPIP Facets come from the </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">TedoneItemAssignmentTable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> spreadsheet containing these items.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Used to validate the input:</t>
@@ -1136,7 +1305,7 @@
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1223,8 +1392,15 @@
     </font>
     <font>
       <b val="true"/>
-      <i val="true"/>
-      <sz val="10"/>
+      <u val="single"/>
+      <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <u val="single"/>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1242,6 +1418,13 @@
     </font>
     <font>
       <sz val="10.5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <u val="single"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1294,7 +1477,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1360,30 +1543,34 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1395,31 +1582,35 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -16141,56 +16332,60 @@
       <c r="D360" s="2"/>
       <c r="E360" s="2"/>
     </row>
-    <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A400" s="16"/>
+    <row r="400" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A400" s="16" t="s">
+        <v>347</v>
+      </c>
       <c r="B400" s="2"/>
       <c r="C400" s="2"/>
       <c r="D400" s="2"/>
       <c r="E400" s="2"/>
     </row>
-    <row r="401" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="17" t="s">
-        <v>347</v>
-      </c>
-      <c r="B401" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C401" s="5"/>
-      <c r="D401" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="E401" s="5" t="s">
+      <c r="B401" s="18" t="s">
         <v>349</v>
       </c>
-      <c r="F401" s="5" t="s">
+      <c r="C401" s="18"/>
+      <c r="D401" s="18" t="s">
         <v>350</v>
       </c>
+      <c r="E401" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="F401" s="18" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="402" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A402" s="18" t="s">
-        <v>351</v>
-      </c>
-      <c r="B402" s="19"/>
-      <c r="C402" s="19"/>
-      <c r="D402" s="20" t="n">
+      <c r="A402" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="B402" s="20"/>
+      <c r="C402" s="20"/>
+      <c r="D402" s="21" t="n">
         <f aca="false">SUM(D403:D408)</f>
         <v>0</v>
       </c>
-      <c r="E402" s="20" t="n">
+      <c r="E402" s="21" t="n">
         <f aca="false">QUOTIENT(PRODUCT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT(D402,60),5),12)</f>
         <v>-25</v>
       </c>
-      <c r="F402" s="21" t="str">
+      <c r="F402" s="22" t="str">
         <f aca="false">IF(E402&lt;=20,"Very Low",IF(E402&lt;=36,"Low",IF(E402&lt;=46,"A Little Low",IF(E402&lt;=53,"Average",IF(E402&lt;=63,"A Little High",IF(E402&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A403" s="22"/>
-      <c r="B403" s="23" t="s">
+      <c r="A403" s="23" t="s">
+        <v>354</v>
+      </c>
+      <c r="B403" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="C403" s="23"/>
+      <c r="C403" s="24"/>
       <c r="D403" s="2" t="n">
         <f aca="false">SUM(AP27+AP48+AP97+AP133+AP168+AP193+AP214+AP228+AP261+AP300)</f>
         <v>0</v>
@@ -16199,17 +16394,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D403,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F403" s="24" t="str">
+      <c r="F403" s="25" t="str">
         <f aca="false">IF(E403&lt;=20,"Very Low",IF(E403&lt;=36,"Low",IF(E403&lt;=46,"A Little Low",IF(E403&lt;=53,"Average",IF(E403&lt;=63,"A Little High",IF(E403&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A404" s="22"/>
-      <c r="B404" s="23" t="s">
+      <c r="A404" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="B404" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C404" s="23"/>
+      <c r="C404" s="24"/>
       <c r="D404" s="2" t="n">
         <f aca="false">SUM(AP14+AP40+AP67+AP102+AP130+AP180+AP202+AP236+AP262+AP288)</f>
         <v>0</v>
@@ -16218,17 +16415,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D404,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F404" s="24" t="str">
+      <c r="F404" s="25" t="str">
         <f aca="false">IF(E404&lt;=20,"Very Low",IF(E404&lt;=36,"Low",IF(E404&lt;=46,"A Little Low",IF(E404&lt;=53,"Average",IF(E404&lt;=63,"A Little High",IF(E404&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A405" s="22"/>
-      <c r="B405" s="23" t="s">
+      <c r="A405" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="B405" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C405" s="23"/>
+      <c r="C405" s="24"/>
       <c r="D405" s="2" t="n">
         <f aca="false">SUM(AP11+AP30+AP78+AP132+AP166+AP196+AP209+AP225+AP246+AP281)</f>
         <v>0</v>
@@ -16237,17 +16436,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D405,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F405" s="24" t="str">
+      <c r="F405" s="25" t="str">
         <f aca="false">IF(E405&lt;=20,"Very Low",IF(E405&lt;=36,"Low",IF(E405&lt;=46,"A Little Low",IF(E405&lt;=53,"Average",IF(E405&lt;=63,"A Little High",IF(E405&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A406" s="22"/>
-      <c r="B406" s="23" t="s">
+      <c r="A406" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="B406" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C406" s="23"/>
+      <c r="C406" s="24"/>
       <c r="D406" s="2" t="n">
         <f aca="false">SUM(AP12+AP49+AP73+AP88+AP111+AP145+AP159+AP204+AP280+AP254)</f>
         <v>0</v>
@@ -16256,17 +16457,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D406,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F406" s="24" t="str">
+      <c r="F406" s="25" t="str">
         <f aca="false">IF(E406&lt;=20,"Very Low",IF(E406&lt;=36,"Low",IF(E406&lt;=46,"A Little Low",IF(E406&lt;=53,"Average",IF(E406&lt;=63,"A Little High",IF(E406&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A407" s="25"/>
-      <c r="B407" s="23" t="s">
+      <c r="A407" s="23" t="s">
+        <v>358</v>
+      </c>
+      <c r="B407" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C407" s="23"/>
+      <c r="C407" s="24"/>
       <c r="D407" s="2" t="n">
         <f aca="false">SUM(AP33+AP62+AP95+AP115+AP128+AP172+AP190+AP215+AP266+AP297)</f>
         <v>0</v>
@@ -16275,17 +16478,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D407,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F407" s="24" t="str">
+      <c r="F407" s="25" t="str">
         <f aca="false">IF(E407&lt;=20,"Very Low",IF(E407&lt;=36,"Low",IF(E407&lt;=46,"A Little Low",IF(E407&lt;=53,"Average",IF(E407&lt;=63,"A Little High",IF(E407&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A408" s="25"/>
-      <c r="B408" s="23" t="s">
+      <c r="A408" s="23" t="s">
+        <v>359</v>
+      </c>
+      <c r="B408" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C408" s="23"/>
+      <c r="C408" s="24"/>
       <c r="D408" s="2" t="n">
         <f aca="false">SUM(AP7+AP24+AP57+AP71+AP192+AP208+AP218+AP251+AP290+AP302)</f>
         <v>0</v>
@@ -16294,44 +16499,46 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D408,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F408" s="24" t="str">
+      <c r="F408" s="25" t="str">
         <f aca="false">IF(E408&lt;=20,"Very Low",IF(E408&lt;=36,"Low",IF(E408&lt;=46,"A Little Low",IF(E408&lt;=53,"Average",IF(E408&lt;=63,"A Little High",IF(E408&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A409" s="25"/>
-      <c r="B409" s="23"/>
+      <c r="A409" s="26"/>
+      <c r="B409" s="24"/>
       <c r="C409" s="10"/>
       <c r="D409" s="2"/>
       <c r="E409" s="2"/>
-      <c r="F409" s="26"/>
+      <c r="F409" s="27"/>
     </row>
     <row r="410" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A410" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="B410" s="19"/>
-      <c r="C410" s="19"/>
-      <c r="D410" s="20" t="n">
+      <c r="A410" s="19" t="s">
+        <v>360</v>
+      </c>
+      <c r="B410" s="20"/>
+      <c r="C410" s="20"/>
+      <c r="D410" s="21" t="n">
         <f aca="false">SUM(D411:D416)</f>
         <v>0</v>
       </c>
-      <c r="E410" s="20" t="n">
+      <c r="E410" s="21" t="n">
         <f aca="false">QUOTIENT(PRODUCT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT(D410,60),5),12)</f>
         <v>-25</v>
       </c>
-      <c r="F410" s="21" t="str">
+      <c r="F410" s="22" t="str">
         <f aca="false">IF(E410&lt;=20,"Very Low",IF(E410&lt;=36,"Low",IF(E410&lt;=46,"A Little Low",IF(E410&lt;=53,"Average",IF(E410&lt;=63,"A Little High",IF(E410&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A411" s="25"/>
-      <c r="B411" s="23" t="s">
+      <c r="A411" s="23" t="s">
+        <v>361</v>
+      </c>
+      <c r="B411" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C411" s="23"/>
+      <c r="C411" s="24"/>
       <c r="D411" s="2" t="n">
         <f aca="false">SUM(AP18+AP50+AP80+AP96+AP112+AP129+AP171+AP212+AP260+AP287)</f>
         <v>0</v>
@@ -16340,17 +16547,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D411,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F411" s="24" t="str">
+      <c r="F411" s="25" t="str">
         <f aca="false">IF(E411&lt;=20,"Very Low",IF(E411&lt;=36,"Low",IF(E411&lt;=46,"A Little Low",IF(E411&lt;=53,"Average",IF(E411&lt;=63,"A Little High",IF(E411&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A412" s="25"/>
-      <c r="B412" s="23" t="s">
+      <c r="A412" s="23" t="s">
+        <v>362</v>
+      </c>
+      <c r="B412" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="C412" s="23"/>
+      <c r="C412" s="24"/>
       <c r="D412" s="2" t="n">
         <f aca="false">SUM(AP55+AP72+AP86+AP106+AP122+AP136+AP182+AP220+AP268+AP285)</f>
         <v>0</v>
@@ -16359,17 +16568,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D412,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F412" s="24" t="str">
+      <c r="F412" s="25" t="str">
         <f aca="false">IF(E412&lt;=20,"Very Low",IF(E412&lt;=36,"Low",IF(E412&lt;=46,"A Little Low",IF(E412&lt;=53,"Average",IF(E412&lt;=63,"A Little High",IF(E412&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A413" s="25"/>
-      <c r="B413" s="23" t="s">
+      <c r="A413" s="23" t="s">
+        <v>363</v>
+      </c>
+      <c r="B413" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C413" s="23"/>
+      <c r="C413" s="24"/>
       <c r="D413" s="2" t="n">
         <f aca="false">SUM(AP5+AP38+AP69+AP84+AP104+AP135+AP151+AP223+AP245+AP264)</f>
         <v>0</v>
@@ -16378,17 +16589,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D413,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F413" s="24" t="str">
+      <c r="F413" s="25" t="str">
         <f aca="false">IF(E413&lt;=20,"Very Low",IF(E413&lt;=36,"Low",IF(E413&lt;=46,"A Little Low",IF(E413&lt;=53,"Average",IF(E413&lt;=63,"A Little High",IF(E413&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A414" s="25"/>
-      <c r="B414" s="23" t="s">
+      <c r="A414" s="23" t="s">
+        <v>364</v>
+      </c>
+      <c r="B414" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C414" s="23"/>
+      <c r="C414" s="24"/>
       <c r="D414" s="2" t="n">
         <f aca="false">SUM(AP13+AP32+AP53+AP94+AP150+AP179+AP213+AP227+AP270+AP296)</f>
         <v>0</v>
@@ -16397,17 +16610,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D414,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F414" s="24" t="str">
+      <c r="F414" s="25" t="str">
         <f aca="false">IF(E414&lt;=20,"Very Low",IF(E414&lt;=36,"Low",IF(E414&lt;=46,"A Little Low",IF(E414&lt;=53,"Average",IF(E414&lt;=63,"A Little High",IF(E414&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A415" s="25"/>
-      <c r="B415" s="23" t="s">
+      <c r="A415" s="23" t="s">
+        <v>365</v>
+      </c>
+      <c r="B415" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="C415" s="23"/>
+      <c r="C415" s="24"/>
       <c r="D415" s="2" t="n">
         <f aca="false">SUM(AP26+AP47+AP64+AP87+AP140+AP153+AP188+AP250+AP269+AP289)</f>
         <v>0</v>
@@ -16416,17 +16631,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D415,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F415" s="24" t="str">
+      <c r="F415" s="25" t="str">
         <f aca="false">IF(E415&lt;=20,"Very Low",IF(E415&lt;=36,"Low",IF(E415&lt;=46,"A Little Low",IF(E415&lt;=53,"Average",IF(E415&lt;=63,"A Little High",IF(E415&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A416" s="25"/>
-      <c r="B416" s="23" t="s">
+      <c r="A416" s="23" t="s">
+        <v>366</v>
+      </c>
+      <c r="B416" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C416" s="23"/>
+      <c r="C416" s="24"/>
       <c r="D416" s="2" t="n">
         <f aca="false">SUM(AP25+AP61+AP113+AP147+AP164+AP187+AP211+AP243+AP272+AP292)</f>
         <v>0</v>
@@ -16435,44 +16652,46 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D416,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F416" s="24" t="str">
+      <c r="F416" s="25" t="str">
         <f aca="false">IF(E416&lt;=20,"Very Low",IF(E416&lt;=36,"Low",IF(E416&lt;=46,"A Little Low",IF(E416&lt;=53,"Average",IF(E416&lt;=63,"A Little High",IF(E416&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A417" s="25"/>
-      <c r="B417" s="23"/>
+      <c r="A417" s="26"/>
+      <c r="B417" s="24"/>
       <c r="C417" s="10"/>
       <c r="D417" s="2"/>
       <c r="E417" s="2"/>
-      <c r="F417" s="26"/>
+      <c r="F417" s="27"/>
     </row>
     <row r="418" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A418" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="B418" s="27"/>
-      <c r="C418" s="27"/>
-      <c r="D418" s="20" t="n">
+      <c r="A418" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="B418" s="28"/>
+      <c r="C418" s="28"/>
+      <c r="D418" s="21" t="n">
         <f aca="false">SUM(D419:D424)</f>
         <v>0</v>
       </c>
-      <c r="E418" s="20" t="n">
+      <c r="E418" s="21" t="n">
         <f aca="false">QUOTIENT(PRODUCT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT(D418,60),5),12)</f>
         <v>-25</v>
       </c>
-      <c r="F418" s="21" t="str">
+      <c r="F418" s="22" t="str">
         <f aca="false">IF(E418&lt;=20,"Very Low",IF(E418&lt;=36,"Low",IF(E418&lt;=46,"A Little Low",IF(E418&lt;=53,"Average",IF(E418&lt;=63,"A Little High",IF(E418&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A419" s="25"/>
-      <c r="B419" s="23" t="s">
+      <c r="A419" s="23" t="s">
+        <v>368</v>
+      </c>
+      <c r="B419" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C419" s="23"/>
+      <c r="C419" s="24"/>
       <c r="D419" s="2" t="n">
         <f aca="false">SUM(AP28+AP45+AP103+AP120+AP137+AP152+AP173+AP221+AP248+AP294)</f>
         <v>0</v>
@@ -16481,17 +16700,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D419,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F419" s="24" t="str">
+      <c r="F419" s="25" t="str">
         <f aca="false">IF(E419&lt;=20,"Very Low",IF(E419&lt;=36,"Low",IF(E419&lt;=46,"A Little Low",IF(E419&lt;=53,"Average",IF(E419&lt;=63,"A Little High",IF(E419&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A420" s="25"/>
-      <c r="B420" s="23" t="s">
+      <c r="A420" s="23" t="s">
+        <v>369</v>
+      </c>
+      <c r="B420" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C420" s="23"/>
+      <c r="C420" s="24"/>
       <c r="D420" s="2" t="n">
         <f aca="false">SUM(AP22+AP52+AP98+AP126+AP144+AP176+AP195+AP226+AP252+AP265)</f>
         <v>0</v>
@@ -16500,17 +16721,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D420,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F420" s="24" t="str">
+      <c r="F420" s="25" t="str">
         <f aca="false">IF(E420&lt;=20,"Very Low",IF(E420&lt;=36,"Low",IF(E420&lt;=46,"A Little Low",IF(E420&lt;=53,"Average",IF(E420&lt;=63,"A Little High",IF(E420&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A421" s="25"/>
-      <c r="B421" s="23" t="s">
+      <c r="A421" s="23" t="s">
+        <v>370</v>
+      </c>
+      <c r="B421" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="C421" s="23"/>
+      <c r="C421" s="24"/>
       <c r="D421" s="2" t="n">
         <f aca="false">SUM(AP29+AP59+AP105+AP124+AP148+AP181+AP200+AP219+AP233+AP244)</f>
         <v>0</v>
@@ -16519,17 +16742,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D421,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F421" s="24" t="str">
+      <c r="F421" s="25" t="str">
         <f aca="false">IF(E421&lt;=20,"Very Low",IF(E421&lt;=36,"Low",IF(E421&lt;=46,"A Little Low",IF(E421&lt;=53,"Average",IF(E421&lt;=63,"A Little High",IF(E421&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A422" s="25"/>
-      <c r="B422" s="23" t="s">
+      <c r="A422" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="B422" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C422" s="23"/>
+      <c r="C422" s="24"/>
       <c r="D422" s="2" t="n">
         <f aca="false">SUM(AP41+AP77+AP114+AP158+AP186+AP206+AP224+AP258+AP275+AP293)</f>
         <v>0</v>
@@ -16538,17 +16763,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D422,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F422" s="24" t="str">
+      <c r="F422" s="25" t="str">
         <f aca="false">IF(E422&lt;=20,"Very Low",IF(E422&lt;=36,"Low",IF(E422&lt;=46,"A Little Low",IF(E422&lt;=53,"Average",IF(E422&lt;=63,"A Little High",IF(E422&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A423" s="25"/>
-      <c r="B423" s="23" t="s">
+      <c r="A423" s="23" t="s">
+        <v>372</v>
+      </c>
+      <c r="B423" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C423" s="23"/>
+      <c r="C423" s="24"/>
       <c r="D423" s="2" t="n">
         <f aca="false">SUM(AP16+AP44+AP66+AP110+AP143+AP163+AP199+AP232+AP256+AP282)</f>
         <v>0</v>
@@ -16557,17 +16784,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D423,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F423" s="24" t="str">
+      <c r="F423" s="25" t="str">
         <f aca="false">IF(E423&lt;=20,"Very Low",IF(E423&lt;=36,"Low",IF(E423&lt;=46,"A Little Low",IF(E423&lt;=53,"Average",IF(E423&lt;=63,"A Little High",IF(E423&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A424" s="25"/>
-      <c r="B424" s="23" t="s">
+      <c r="A424" s="23" t="s">
+        <v>373</v>
+      </c>
+      <c r="B424" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C424" s="23"/>
+      <c r="C424" s="24"/>
       <c r="D424" s="2" t="n">
         <f aca="false">SUM(AP6+AP37+AP60+AP99+AP116+AP160+AP210+AP240+AP274+AP301)</f>
         <v>0</v>
@@ -16576,44 +16805,46 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D424,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F424" s="24" t="str">
+      <c r="F424" s="25" t="str">
         <f aca="false">IF(E424&lt;=20,"Very Low",IF(E424&lt;=36,"Low",IF(E424&lt;=46,"A Little Low",IF(E424&lt;=53,"Average",IF(E424&lt;=63,"A Little High",IF(E424&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A425" s="25"/>
-      <c r="B425" s="23"/>
+      <c r="A425" s="26"/>
+      <c r="B425" s="24"/>
       <c r="C425" s="10"/>
-      <c r="D425" s="20"/>
-      <c r="E425" s="20"/>
-      <c r="F425" s="28"/>
+      <c r="D425" s="21"/>
+      <c r="E425" s="21"/>
+      <c r="F425" s="29"/>
     </row>
     <row r="426" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A426" s="29" t="s">
-        <v>354</v>
-      </c>
-      <c r="B426" s="30"/>
-      <c r="C426" s="30"/>
-      <c r="D426" s="20" t="n">
+      <c r="A426" s="30" t="s">
+        <v>374</v>
+      </c>
+      <c r="B426" s="31"/>
+      <c r="C426" s="31"/>
+      <c r="D426" s="21" t="n">
         <f aca="false">SUM(D427:D432)</f>
         <v>0</v>
       </c>
-      <c r="E426" s="20" t="n">
+      <c r="E426" s="21" t="n">
         <f aca="false">QUOTIENT(PRODUCT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT(D426,60),5),12)</f>
         <v>-25</v>
       </c>
-      <c r="F426" s="21" t="str">
+      <c r="F426" s="22" t="str">
         <f aca="false">IF(E426&lt;=20,"Very Low",IF(E426&lt;=36,"Low",IF(E426&lt;=46,"A Little Low",IF(E426&lt;=53,"Average",IF(E426&lt;=63,"A Little High",IF(E426&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A427" s="25"/>
-      <c r="B427" s="23" t="s">
+      <c r="A427" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="B427" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C427" s="23"/>
+      <c r="C427" s="24"/>
       <c r="D427" s="2" t="n">
         <f aca="false">SUM(AP15+AP34+AP56+AP74+AP90+AP146+AP177+AP198+AP239+AP291)</f>
         <v>0</v>
@@ -16622,17 +16853,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D427,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F427" s="24" t="str">
+      <c r="F427" s="25" t="str">
         <f aca="false">IF(E427&lt;=20,"Very Low",IF(E427&lt;=36,"Low",IF(E427&lt;=46,"A Little Low",IF(E427&lt;=53,"Average",IF(E427&lt;=63,"A Little High",IF(E427&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A428" s="25"/>
-      <c r="B428" s="23" t="s">
+      <c r="A428" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="B428" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C428" s="23"/>
+      <c r="C428" s="24"/>
       <c r="D428" s="2" t="n">
         <f aca="false">SUM(AP51+AP76+AP101+AP123+AP142+AP170+AP184+AP231+AP249+AP276)</f>
         <v>0</v>
@@ -16641,17 +16874,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D428,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F428" s="24" t="str">
+      <c r="F428" s="25" t="str">
         <f aca="false">IF(E428&lt;=20,"Very Low",IF(E428&lt;=36,"Low",IF(E428&lt;=46,"A Little Low",IF(E428&lt;=53,"Average",IF(E428&lt;=63,"A Little High",IF(E428&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A429" s="25"/>
-      <c r="B429" s="23" t="s">
+      <c r="A429" s="23" t="s">
+        <v>377</v>
+      </c>
+      <c r="B429" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C429" s="23"/>
+      <c r="C429" s="24"/>
       <c r="D429" s="2" t="n">
         <f aca="false">SUM(AP8+AP58+AP85+AP131+AP156+AP178+AP205+AP234+AP267+AP286)</f>
         <v>0</v>
@@ -16660,17 +16895,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D429,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F429" s="24" t="str">
+      <c r="F429" s="25" t="str">
         <f aca="false">IF(E429&lt;=20,"Very Low",IF(E429&lt;=36,"Low",IF(E429&lt;=46,"A Little Low",IF(E429&lt;=53,"Average",IF(E429&lt;=63,"A Little High",IF(E429&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A430" s="25"/>
-      <c r="B430" s="23" t="s">
+      <c r="A430" s="23" t="s">
+        <v>378</v>
+      </c>
+      <c r="B430" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C430" s="23"/>
+      <c r="C430" s="24"/>
       <c r="D430" s="2" t="n">
         <f aca="false">SUM(AP10+AP39+AP68+AP91+AP125+AP149+AP161+AP229+AP263+AP284)</f>
         <v>0</v>
@@ -16679,17 +16916,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D430,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F430" s="24" t="str">
+      <c r="F430" s="25" t="str">
         <f aca="false">IF(E430&lt;=20,"Very Low",IF(E430&lt;=36,"Low",IF(E430&lt;=46,"A Little Low",IF(E430&lt;=53,"Average",IF(E430&lt;=63,"A Little High",IF(E430&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A431" s="25"/>
-      <c r="B431" s="23" t="s">
+      <c r="A431" s="23" t="s">
+        <v>379</v>
+      </c>
+      <c r="B431" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="C431" s="23"/>
+      <c r="C431" s="24"/>
       <c r="D431" s="2" t="n">
         <f aca="false">SUM(AP54+AP83+AP121+AP141+AP165+AP183+AP201+AP216+AP271+AP303)</f>
         <v>0</v>
@@ -16698,17 +16937,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D431,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F431" s="24" t="str">
+      <c r="F431" s="25" t="str">
         <f aca="false">IF(E431&lt;=20,"Very Low",IF(E431&lt;=36,"Low",IF(E431&lt;=46,"A Little Low",IF(E431&lt;=53,"Average",IF(E431&lt;=63,"A Little High",IF(E431&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A432" s="25"/>
-      <c r="B432" s="23" t="s">
+      <c r="A432" s="23" t="s">
+        <v>380</v>
+      </c>
+      <c r="B432" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C432" s="23"/>
+      <c r="C432" s="24"/>
       <c r="D432" s="2" t="n">
         <f aca="false">SUM(AP19+AP42+AP65+AP89+AP127+AP167+AP203+AP230+AP255+AP283)</f>
         <v>0</v>
@@ -16717,41 +16958,43 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D432,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F432" s="24" t="str">
+      <c r="F432" s="25" t="str">
         <f aca="false">IF(E432&lt;=20,"Very Low",IF(E432&lt;=36,"Low",IF(E432&lt;=46,"A Little Low",IF(E432&lt;=53,"Average",IF(E432&lt;=63,"A Little High",IF(E432&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A433" s="25"/>
-      <c r="B433" s="23"/>
+      <c r="A433" s="23"/>
+      <c r="B433" s="24"/>
       <c r="C433" s="10"/>
     </row>
     <row r="434" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A434" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="B434" s="27"/>
-      <c r="C434" s="27"/>
-      <c r="D434" s="20" t="n">
+      <c r="A434" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="B434" s="28"/>
+      <c r="C434" s="28"/>
+      <c r="D434" s="21" t="n">
         <f aca="false">SUM(D435:D440)</f>
         <v>0</v>
       </c>
-      <c r="E434" s="20" t="n">
+      <c r="E434" s="21" t="n">
         <f aca="false">QUOTIENT(PRODUCT(_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT(D434,60),5),12)</f>
         <v>-25</v>
       </c>
-      <c r="F434" s="21" t="str">
+      <c r="F434" s="22" t="str">
         <f aca="false">IF(E434&lt;=20,"Very Low",IF(E434&lt;=36,"Low",IF(E434&lt;=46,"A Little Low",IF(E434&lt;=53,"Average",IF(E434&lt;=63,"A Little High",IF(E434&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A435" s="25"/>
-      <c r="B435" s="23" t="s">
+      <c r="A435" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="B435" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C435" s="23"/>
+      <c r="C435" s="24"/>
       <c r="D435" s="2" t="n">
         <f aca="false">SUM(AP17+AP46+AP75+AP93+AP134+AP175+AP241+AP257+AP279+AP299)</f>
         <v>0</v>
@@ -16760,17 +17003,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D435,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F435" s="24" t="str">
+      <c r="F435" s="25" t="str">
         <f aca="false">IF(E435&lt;=20,"Very Low",IF(E435&lt;=36,"Low",IF(E435&lt;=46,"A Little Low",IF(E435&lt;=53,"Average",IF(E435&lt;=63,"A Little High",IF(E435&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A436" s="25"/>
-      <c r="B436" s="23" t="s">
+      <c r="A436" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="B436" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C436" s="23"/>
+      <c r="C436" s="24"/>
       <c r="D436" s="2" t="n">
         <f aca="false">SUM(AP21+AP36+AP70+AP109+AP138+AP155+AP189+AP207+AP235+AP277)</f>
         <v>0</v>
@@ -16779,17 +17024,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D436,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F436" s="24" t="str">
+      <c r="F436" s="25" t="str">
         <f aca="false">IF(E436&lt;=20,"Very Low",IF(E436&lt;=36,"Low",IF(E436&lt;=46,"A Little Low",IF(E436&lt;=53,"Average",IF(E436&lt;=63,"A Little High",IF(E436&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A437" s="25"/>
-      <c r="B437" s="23" t="s">
+      <c r="A437" s="23" t="s">
+        <v>384</v>
+      </c>
+      <c r="B437" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="C437" s="23"/>
+      <c r="C437" s="24"/>
       <c r="D437" s="2" t="n">
         <f aca="false">SUM(AP31+AP82+AP100+AP119+AP139+AP162+AP191+AP247+AP278+AP304)</f>
         <v>0</v>
@@ -16798,17 +17045,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D437,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F437" s="24" t="str">
+      <c r="F437" s="25" t="str">
         <f aca="false">IF(E437&lt;=20,"Very Low",IF(E437&lt;=36,"Low",IF(E437&lt;=46,"A Little Low",IF(E437&lt;=53,"Average",IF(E437&lt;=63,"A Little High",IF(E437&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A438" s="25"/>
-      <c r="B438" s="23" t="s">
+      <c r="A438" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="B438" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C438" s="23"/>
+      <c r="C438" s="24"/>
       <c r="D438" s="2" t="n">
         <f aca="false">SUM(AP9+AP35+AP63+AP92+AP118+AP169+AP197+AP237+AP253+AP298)</f>
         <v>0</v>
@@ -16817,17 +17066,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D438,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F438" s="24" t="str">
+      <c r="F438" s="25" t="str">
         <f aca="false">IF(E438&lt;=20,"Very Low",IF(E438&lt;=36,"Low",IF(E438&lt;=46,"A Little Low",IF(E438&lt;=53,"Average",IF(E438&lt;=63,"A Little High",IF(E438&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A439" s="25"/>
-      <c r="B439" s="23" t="s">
+      <c r="A439" s="23" t="s">
+        <v>386</v>
+      </c>
+      <c r="B439" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C439" s="23"/>
+      <c r="C439" s="24"/>
       <c r="D439" s="2" t="n">
         <f aca="false">SUM(AP23+AP81+AP108+AP154+AP174+AP194+AP217+AP242+AP273+AP295)</f>
         <v>0</v>
@@ -16836,17 +17087,19 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D439,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F439" s="24" t="str">
+      <c r="F439" s="25" t="str">
         <f aca="false">IF(E439&lt;=20,"Very Low",IF(E439&lt;=36,"Low",IF(E439&lt;=46,"A Little Low",IF(E439&lt;=53,"Average",IF(E439&lt;=63,"A Little High",IF(E439&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A440" s="25"/>
-      <c r="B440" s="23" t="s">
+      <c r="A440" s="23" t="s">
+        <v>387</v>
+      </c>
+      <c r="B440" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C440" s="23"/>
+      <c r="C440" s="24"/>
       <c r="D440" s="2" t="n">
         <f aca="false">SUM(AP20+AP43+AP79+AP107+AP117+AP157+AP185+AP222+AP238+AP259)</f>
         <v>0</v>
@@ -16855,7 +17108,7 @@
         <f aca="false">QUOTIENT(PRODUCT(5,_xlfn.ORG.LIBREOFFICE.RAWSUBTRACT( D440,10)),2)</f>
         <v>-25</v>
       </c>
-      <c r="F440" s="24" t="str">
+      <c r="F440" s="25" t="str">
         <f aca="false">IF(E440&lt;=20,"Very Low",IF(E440&lt;=36,"Low",IF(E440&lt;=46,"A Little Low",IF(E440&lt;=53,"Average",IF(E440&lt;=63,"A Little High",IF(E440&lt;=79,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
@@ -16867,12 +17120,18 @@
       <c r="E441" s="2"/>
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A442" s="32" t="s">
+        <v>388</v>
+      </c>
       <c r="B442" s="2"/>
       <c r="C442" s="2"/>
       <c r="D442" s="2"/>
       <c r="E442" s="2"/>
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A443" s="10" t="s">
+        <v>389</v>
+      </c>
       <c r="B443" s="2"/>
       <c r="C443" s="2"/>
       <c r="D443" s="2"/>
@@ -17065,14 +17324,14 @@
       <c r="E474" s="2"/>
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A475" s="31" t="s">
-        <v>356</v>
+      <c r="A475" s="33" t="s">
+        <v>390</v>
       </c>
       <c r="B475" s="2" t="s">
-        <v>357</v>
+        <v>391</v>
       </c>
       <c r="C475" s="2" t="s">
-        <v>358</v>
+        <v>392</v>
       </c>
       <c r="D475" s="2"/>
       <c r="E475" s="2"/>
@@ -18501,7 +18760,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>359</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>